<commit_message>
Updated CYRS Review Decisions
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_CYRS_Review.xlsx
+++ b/Input Documents/PO3_DGW_CYRS_Review.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20354"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA9A8FB-BC02-4C7C-9831-B361B738182B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12546B6F-509D-48F2-8CC6-74961795BC3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -177,15 +177,6 @@
 - When mode is time watch , hours , mintues , and AM/PM can be adjusted and select between them with selection button "Func1"
 - When mintue is selected and increment button is pressed "Func2" it should be incremented by 1 
 - and so on like this </t>
-  </si>
-  <si>
-    <t>Not clear and modification has been done upon the undersanding of the point (Removed hardware reqirments section)</t>
-  </si>
-  <si>
-    <t>Confilect  with Point 9</t>
-  </si>
-  <si>
-    <t>Confilect  with Point 7 and 8</t>
   </si>
 </sst>
 </file>
@@ -556,12 +547,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,33 +594,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -961,206 +952,189 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="24" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="33"/>
+      <c r="E12" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="33"/>
+      <c r="G12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="30"/>
+      <c r="G13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1177,6 +1151,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1187,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1364,9 +1355,7 @@
       <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
@@ -1388,14 +1377,12 @@
         <v>46</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="I7" s="12"/>
       <c r="K7" t="s">
         <v>19</v>
       </c>
@@ -1420,14 +1407,12 @@
         <v>47</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>50</v>
-      </c>
+      <c r="I8" s="12"/>
       <c r="K8" t="s">
         <v>22</v>
       </c>
@@ -1452,14 +1437,12 @@
         <v>48</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>51</v>
-      </c>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
@@ -1911,7 +1894,7 @@
       <formula>$G$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$4:$K$5</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Fixed CYRS version date error. Updated CYRS review sheet.
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_CYRS_Review.xlsx
+++ b/Input Documents/PO3_DGW_CYRS_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8B4AA8-5191-40D4-8328-042032062E55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -183,11 +184,14 @@
   <si>
     <t xml:space="preserve">Add one point and update the status for each req </t>
   </si>
+  <si>
+    <t>9/2/2020 - Mariam El-Shakafi: Hardware constraints section was moved to HSI document. Is this point still an issue?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -552,12 +556,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -571,44 +605,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -946,7 +950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -960,96 +964,96 @@
   <sheetData>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="38"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="39"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29"/>
     </row>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="39"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="29"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="40">
+      <c r="C9" s="25"/>
+      <c r="D9" s="32">
         <v>44076</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="33" t="s">
@@ -1083,91 +1087,74 @@
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="30"/>
+      <c r="G13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="31"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>0.2</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="40">
+      <c r="D14" s="30"/>
+      <c r="E14" s="32">
         <v>44076</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
+      <c r="F14" s="30"/>
+      <c r="G14" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="25"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1184,6 +1171,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1191,11 +1195,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,7 +1375,9 @@
       <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
@@ -1479,7 +1485,9 @@
       <c r="F10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="10"/>
+      <c r="G10" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H10" s="10" t="s">
         <v>19</v>
       </c>
@@ -1925,10 +1933,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$7:$K$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Upate SIQ and reveiw sheet
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_CYRS_Review.xlsx
+++ b/Input Documents/PO3_DGW_CYRS_Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8B4AA8-5191-40D4-8328-042032062E55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -187,11 +186,17 @@
   <si>
     <t>9/2/2020 - Mariam El-Shakafi: Hardware constraints section was moved to HSI document. Is this point still an issue?</t>
   </si>
+  <si>
+    <t>23/2/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update resolved points </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -556,12 +561,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,46 +611,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -950,211 +955,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="32">
-        <v>44076</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0.2</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="32">
+      <c r="D14" s="24"/>
+      <c r="E14" s="31">
         <v>44076</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1171,23 +1201,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1195,27 +1208,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1244,7 +1257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -1271,7 +1284,7 @@
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="13"/>
@@ -1290,7 +1303,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -1320,7 +1333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1350,7 +1363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1373,13 +1386,13 @@
         <v>20</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I6" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1409,7 +1422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1439,7 +1452,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
@@ -1466,7 +1479,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>44076</v>
       </c>
@@ -1489,11 +1502,11 @@
         <v>20</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1510,7 +1523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1527,7 +1540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1538,7 +1551,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1549,7 +1562,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="13"/>
@@ -1560,7 +1573,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1571,7 +1584,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
@@ -1582,7 +1595,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1593,7 +1606,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1604,7 +1617,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1615,7 +1628,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1626,7 +1639,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1637,7 +1650,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1648,7 +1661,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1659,7 +1672,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1670,7 +1683,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1681,7 +1694,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
@@ -1692,7 +1705,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1703,7 +1716,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1714,7 +1727,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1725,7 +1738,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1736,7 +1749,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1747,7 +1760,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1758,7 +1771,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1769,7 +1782,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1780,7 +1793,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1791,7 +1804,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1802,7 +1815,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1813,7 +1826,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1824,7 +1837,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1835,7 +1848,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1846,7 +1859,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1857,7 +1870,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1868,7 +1881,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1879,7 +1892,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1890,7 +1903,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -1901,7 +1914,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -1933,10 +1946,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>$K$7:$K$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added review points for CYRS V0.5
Signed-off-by: mariam-elshakafi <mariam.elshakafi@gmail.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_CYRS_Review.xlsx
+++ b/Input Documents/PO3_DGW_CYRS_Review.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94440DE1-4A8C-4C87-9C7B-010E01BE0A3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -41,9 +42,6 @@
   </si>
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>Auther</t>
   </si>
   <si>
     <t xml:space="preserve">Date </t>
@@ -192,15 +190,165 @@
   <si>
     <t xml:space="preserve">Update resolved points </t>
   </si>
+  <si>
+    <t>Mariam</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Mariam El-Shakafi</t>
+  </si>
+  <si>
+    <t>28/2/2020</t>
+  </si>
+  <si>
+    <t>V0.5</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>3.1.6, 3.1.7</t>
+  </si>
+  <si>
+    <t>Merge those into 1 requirement:
+In Display Time mode, when hours’ field is selected, FUNC2 button is used to increment hours up to 12 then back to 1.</t>
+  </si>
+  <si>
+    <t>3.1.8, 3.1.9</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>3.1.10, 3.1.11</t>
+  </si>
+  <si>
+    <t>3.1.16, 3.1.17</t>
+  </si>
+  <si>
+    <t>3.1.18, 3.1.19</t>
+  </si>
+  <si>
+    <t>3.1.20, 3.1.21</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The user cannot adjust time in any mode (only in display time mode). So, remove this requirement. Instead, use 2 requirements:
+- If MODE button is pressed while adjusting time in display time mode, changes should be saved and user shall return to display time mode. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(replacing req. 3.1.13)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- If MODE button is pressed while setting alarm in alarm time mode, alarm settings should be saved and user shall return to display time mode. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(replacing req. 3.1.23)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>3.1.24</t>
+  </si>
+  <si>
+    <t>Add a requirement to disable alarm. Add a requirement for the initial state of alarm (which is disabled according to SIQ).</t>
+  </si>
+  <si>
+    <r>
+      <t>Remove this requirement (Instead: edit requirement</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 3.1.26 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>which has the same meaning).</t>
+    </r>
+  </si>
+  <si>
+    <t>3.1.14</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">According to SIQ, when user changes mode to alarm, they'll immediately be taken to setting alarm. Hence, this requirement is not valid. Instead, it should mention:
+The system shows the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>alarm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> time in HH:MM:SS AM/PM format when current mode is Display Time mode and mode is changed.</t>
+    </r>
+  </si>
+  <si>
+    <t>Added review points to CYRS V0.5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +416,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -561,12 +729,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -581,43 +779,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="2"/>
+    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -955,236 +1123,227 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="32" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="39"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="37"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="40"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="40"/>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="32" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="36"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="36"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>0.2</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="31">
+      <c r="C14" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="32">
         <v>44076</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="30"/>
+      <c r="G14" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>0.3</v>
       </c>
-      <c r="C15" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24" t="s">
+      <c r="C15" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1201,6 +1360,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1208,427 +1384,567 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" customWidth="1"/>
-    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" customWidth="1"/>
+    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="F2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="13"/>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>41</v>
-      </c>
       <c r="G4" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="10"/>
       <c r="K4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="D5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="10"/>
       <c r="K5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="I6" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="9" t="s">
-        <v>45</v>
-      </c>
       <c r="G7" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="12"/>
       <c r="K7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="H8" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" s="12"/>
       <c r="K8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>37</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>44076</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="G10" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
+    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="H11" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I11" s="12"/>
       <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
         <v>23</v>
       </c>
-      <c r="L11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="H12" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I12" s="12"/>
       <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
         <v>25</v>
       </c>
-      <c r="L12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="H13" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="H14" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="H15" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="H16" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="18"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>70</v>
+      </c>
       <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="H18" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>69</v>
+      </c>
       <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="H19" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
+    <row r="20" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="H20" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1639,7 +1955,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1650,7 +1966,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1661,7 +1977,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1672,7 +1988,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1683,7 +1999,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1694,7 +2010,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
@@ -1705,7 +2021,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -1716,7 +2032,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1727,7 +2043,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1738,7 +2054,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -1749,7 +2065,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1760,7 +2076,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -1771,7 +2087,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -1782,7 +2098,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1793,7 +2109,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1804,7 +2120,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1815,7 +2131,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1826,7 +2142,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1837,7 +2153,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1848,7 +2164,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1859,7 +2175,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1870,7 +2186,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1881,7 +2197,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1892,7 +2208,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1903,7 +2219,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -1914,7 +2230,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -1926,6 +2242,7 @@
       <c r="I47" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="G1">
     <cfRule type="cellIs" dxfId="4" priority="18" stopIfTrue="1" operator="equal">
       <formula>$G$4</formula>
@@ -1946,10 +2263,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$K$7:$K$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update CYRS to cover review points Signed-off-by: AmrElnobe <ibrahimamr222@hotmial.com>
</commit_message>
<xml_diff>
--- a/Input Documents/PO3_DGW_CYRS_Review.xlsx
+++ b/Input Documents/PO3_DGW_CYRS_Review.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94440DE1-4A8C-4C87-9C7B-010E01BE0A3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="74">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -344,7 +343,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -729,12 +728,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -746,46 +778,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3 2" xfId="3"/>
+    <cellStyle name="Normal 4" xfId="2"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -1123,227 +1122,244 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17:H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="40"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="33"/>
+      <c r="D8" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="33"/>
+      <c r="D9" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="33" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="35"/>
+      <c r="E12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0.2</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="32">
+      <c r="D14" s="24"/>
+      <c r="E14" s="31">
         <v>44076</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>0.3</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30" t="s">
+      <c r="F15" s="24"/>
+      <c r="G15" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>0.4</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30" t="s">
+      <c r="F16" s="24"/>
+      <c r="G16" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="37"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1360,23 +1376,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1384,27 +1383,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
@@ -1460,7 +1459,7 @@
       </c>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="13"/>
@@ -1479,7 +1478,7 @@
       </c>
       <c r="I3" s="10"/>
     </row>
-    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>35</v>
       </c>
@@ -1509,7 +1508,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>35</v>
       </c>
@@ -1598,7 +1597,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
@@ -1628,7 +1627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>35</v>
       </c>
@@ -1655,7 +1654,7 @@
       </c>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>44076</v>
       </c>
@@ -1682,7 +1681,7 @@
       </c>
       <c r="I10" s="12"/>
     </row>
-    <row r="11" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>56</v>
       </c>
@@ -1701,9 +1700,11 @@
       <c r="F11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="10"/>
+      <c r="G11" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I11" s="12"/>
       <c r="K11" t="s">
@@ -1713,7 +1714,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>56</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>56</v>
       </c>
@@ -1763,13 +1764,15 @@
       <c r="F13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G13" s="10"/>
+      <c r="G13" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H13" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>56</v>
       </c>
@@ -1788,13 +1791,15 @@
       <c r="F14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H14" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>56</v>
       </c>
@@ -1813,13 +1818,15 @@
       <c r="F15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="10"/>
+      <c r="G15" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H15" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>56</v>
       </c>
@@ -1838,13 +1845,15 @@
       <c r="F16" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="10"/>
+      <c r="G16" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H16" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
@@ -1863,13 +1872,15 @@
       <c r="F17" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G17" s="10"/>
+      <c r="G17" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H17" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>56</v>
       </c>
@@ -1888,13 +1899,15 @@
       <c r="F18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="10"/>
+      <c r="G18" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H18" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>56</v>
       </c>
@@ -1913,13 +1926,15 @@
       <c r="F19" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="10"/>
+      <c r="G19" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H19" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>56</v>
       </c>
@@ -1938,13 +1953,15 @@
       <c r="F20" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="10"/>
+      <c r="G20" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="H20" s="10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1955,7 +1972,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1966,7 +1983,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1977,7 +1994,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1988,7 +2005,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1999,7 +2016,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -2010,7 +2027,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
@@ -2021,7 +2038,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2032,7 +2049,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -2043,7 +2060,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -2054,7 +2071,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -2065,7 +2082,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -2076,7 +2093,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -2087,7 +2104,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
@@ -2098,7 +2115,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -2109,7 +2126,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -2120,7 +2137,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -2131,7 +2148,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -2142,7 +2159,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -2153,7 +2170,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -2164,7 +2181,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -2175,7 +2192,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -2186,7 +2203,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -2197,7 +2214,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -2208,7 +2225,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -2219,7 +2236,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -2230,7 +2247,7 @@
       <c r="H46" s="10"/>
       <c r="I46" s="19"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="16"/>
@@ -2263,10 +2280,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
       <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
       <formula1>$K$7:$K$8</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>